<commit_message>
updates to template and vds
</commit_message>
<xml_diff>
--- a/ChatGPT_Messages/Vector_DB/Question_Query_Embeddings-0.xlsx
+++ b/ChatGPT_Messages/Vector_DB/Question_Query_Embeddings-0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dovcohen/Documents/Projects/AI/NL2SQL/ChatGPT/Vector_DB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dovcohen/Documents/Projects/AI/NL2SQL/ChatGPT_Messages/Vector_DB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B97E0EC-36E3-C14D-BCA7-B7E763D238AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488A9A5D-6AE9-7841-8920-1780AD655699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VDS" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Question</t>
   </si>
@@ -46,12 +46,6 @@
     <t>select  client.Name, address.Address, address.City, address.State, address.Zip FROM client INNER JOIN address ON client.Address_ID = address.ID  WHERE address.City = 'San Diego';</t>
   </si>
   <si>
-    <t>What is Angelica James portfolio summary on 10-11-2023?</t>
-  </si>
-  <si>
-    <t>SELECT product.type AS account_type,  COUNT(CASE WHEN account.status = 'Open' THEN 1 END) AS open_accounts, COUNT(CASE WHEN account.status = 'Closed' THEN 1 END) AS closed_accounts, SUM(balance.balance) AS total_balances, AVG(balance.balance) AS month_to_date_avg_balance FROM account INNER JOIN product ON account.product_id = product.id INNER JOIN balance ON account.id balance.account_id INNER JOIN date ON balance.balance_dt_id = date.id INNER JOIN relationship ON account.id = relationship.account_id INNER JOIN client ON relationship.client_id = client.id  WHERE client.name = 'Angelica James'  AND date.date = '2023-10-11'  AND relationship.relationship_type = 'Primary'  GROUP BY product.type;</t>
-  </si>
-  <si>
     <t>Which clients are members of Angelica James household?</t>
   </si>
   <si>
@@ -68,13 +62,263 @@
   </si>
   <si>
     <t>SELECT client.Name, client.ID, employer.Name, address.Address, address.City, address.State, address.Zip FROM client INNER JOIN employer ON client.Employer_ID = employer.ID INNER JOIN address ON client.Address_ID = address.ID WHERE employer.Name = 'Stevens Valley School';</t>
+  </si>
+  <si>
+    <t>What is Robert King's account balances?</t>
+  </si>
+  <si>
+    <t>What are Robert King's account balances?</t>
+  </si>
+  <si>
+    <t>What is Robert King's current account balances?</t>
+  </si>
+  <si>
+    <t>What are Robert King's latest account balances?</t>
+  </si>
+  <si>
+    <t>What are Robert King's average monthly balances?</t>
+  </si>
+  <si>
+    <t>SELECT date.Month, date.Year, product.Type, account.acct_nbr, avg(balance.Balance) as Avg_Balance
+FROM client
+INNER JOIN relationship ON client.ID = relationship.Client_ID
+INNER JOIN account ON relationship.Account_ID = account.ID
+INNER JOIN balance ON account.ID = balance.Account_ID
+INNER JOIN product ON account.Product_ID = product.ID
+INNER JOIN date ON balance.Balance_Dt_Id = date.ID
+WHERE client.Name = 'Robert King' 
+and relationship.Relationship_Type  = 'Primary'
+group by date.Month, date.Year, product.Type, account.acct_nbr
+ORDER BY account.acct_nbr, date.Month, date.Year</t>
+  </si>
+  <si>
+    <t>SELECT date.Date, product.Type, account.acct_nbr, balance.Balance
+FROM client
+INNER JOIN relationship ON client.ID = relationship.Client_ID
+INNER JOIN account ON relationship.Account_ID = account.ID
+INNER JOIN balance ON account.ID = balance.Account_ID
+INNER JOIN product ON account.Product_ID = product.ID
+INNER JOIN date ON balance.Balance_Dt_Id = date.ID
+WHERE client.Name = 'Robert King' 
+and relationship.Relationship_Type  = 'Primary'
+and balance.Balance_Dt_Id = (select max(Balance_Dt_id) from balance)
+ORDER BY date.Date, account.acct_nbr;</t>
+  </si>
+  <si>
+    <t>SELECT date.Date, product.Type, account.acct_nbr, balance.Balance
+FROM client
+INNER JOIN relationship ON client.ID = relationship.Client_ID
+INNER JOIN account ON relationship.Account_ID = account.ID
+INNER JOIN balance ON account.ID = balance.Account_ID
+INNER JOIN product ON account.Product_ID = product.ID
+INNER JOIN date ON balance.Balance_Dt_Id = date.ID
+WHERE client.Name = 'Robert King' 
+and relationship.Relationship_Type  = 'Primary'
+ORDER BY date.Date, account.acct_nbr;</t>
+  </si>
+  <si>
+    <t>SELECT date.Date, product.Type, account.acct_nbr, balance.Balance
+FROM client
+INNER JOIN relationship ON client.ID = relationship.Client_ID
+INNER JOIN account ON relationship.Account_ID = account.ID
+INNER JOIN balance ON account.ID = balance.Account_ID
+INNER JOIN product ON account.Product_ID = product.ID
+INNER JOIN date ON balance.Balance_Dt_Id = date.ID
+WHERE client.Name = 'Robert King'
+and relationship.Relationship_Type  = 'Primary'
+ORDER BY date.Date, account.acct_nbr;</t>
+  </si>
+  <si>
+    <t>How many ACH transactions per month does Robert King make?</t>
+  </si>
+  <si>
+    <t>SELECT date.Month, date.Year, product.Type, account.acct_nbr, transactions.Transaction_Type, 
+count(transactions.Transaction_Type) as cnt, sum(transactions.Transaction_Amount)
+FROM client
+INNER JOIN relationship ON client.ID = relationship.Client_ID
+INNER JOIN account ON relationship.Account_ID = account.ID
+INNER JOIN transactions ON account.id = transactions.Account_ID 
+INNER JOIN product ON account.Product_ID = product.ID
+INNER JOIN date ON transactions.Date_ID  = date.ID
+WHERE client.Name = 'Robert King'
+and transactions.Transaction_Type  = 'ACH'
+and relationship.Relationship_Type  = 'Primary'
+group by date.Month, date.Year, product.Type, account.acct_nbr, transactions.Transaction_Type
+ORDER BY account.acct_nbr, date.Month, date.Year</t>
+  </si>
+  <si>
+    <t>How many transactions per month grouped by transaction_type does Robert King make?</t>
+  </si>
+  <si>
+    <t>How many investment transactions per month does Robert King make?</t>
+  </si>
+  <si>
+    <t>sELECT date.Month, date.Year, product.Type, account.acct_nbr, transactions.Transaction_Purpose , count(transactions.Transaction_Type) as cnt
+, sum(transactions.Transaction_Amount)
+FROM client
+INNER JOIN relationship ON client.ID = relationship.Client_ID
+INNER JOIN account ON relationship.Account_ID = account.ID
+INNER JOIN transactions ON account.id = transactions.Account_ID 
+INNER JOIN product ON account.Product_ID = product.ID
+INNER JOIN date ON transactions.Date_ID  = date.ID
+WHERE client.Name = 'Robert King'
+and relationship.Relationship_Type  = 'Primary'
+group by date.Month, date.Year, product.Type, account.acct_nbr, transactions.Transaction_Purpose
+ORDER BY account.acct_nbr, transactions.Transaction_Purpose, date.Month, date.Year;</t>
+  </si>
+  <si>
+    <t>sELECT date.Month, date.Year, product.Type, account.acct_nbr, transactions.Transaction_Purpose , count(transactions.Transaction_Type) as cnt
+, sum(transactions.Transaction_Amount)
+FROM client
+INNER JOIN relationship ON client.ID = relationship.Client_ID
+INNER JOIN account ON relationship.Account_ID = account.ID
+INNER JOIN transactions ON account.id = transactions.Account_ID 
+INNER JOIN product ON account.Product_ID = product.ID
+INNER JOIN date ON transactions.Date_ID  = date.ID
+WHERE client.Name = 'Robert King'
+and transactions.Transaction_Purpose = 'Investment'
+and relationship.Relationship_Type  = 'Primary'
+group by date.Month, date.Year, product.Type, account.acct_nbr, transactions.Transaction_Purpose
+ORDER BY account.acct_nbr, date.Month, date.Year</t>
+  </si>
+  <si>
+    <t>How many transactions per month grouped by transaction purpose does Robert King make?</t>
+  </si>
+  <si>
+    <t>sELECT date.Month, date.Year, product.Type, account.acct_nbr, transactions.Transaction_Purpose , count(transactions.Transaction_Type) as cnt
+, sum(transactions.Transaction_Amount)
+FROM client
+INNER JOIN relationship ON client.ID = relationship.Client_ID
+INNER JOIN account ON relationship.Account_ID = account.ID
+INNER JOIN transactions ON account.id = transactions.Account_ID 
+INNER JOIN product ON account.Product_ID = product.ID
+INNER JOIN date ON transactions.Date_ID  = date.ID
+WHERE client.Name = 'Robert King'
+and relationship.Relationship_Type  = 'Primary'
+group by date.Month, date.Year, product.Type, account.acct_nbr, transactions.Transaction_Purpose
+ORDER BY account.acct_nbr, transactions.Transaction_Purpose, date.Month, date.Year</t>
+  </si>
+  <si>
+    <t>with CTE_Latest_Dt as
+(
+select distinct date.date, date.month, date.year
+from balance 
+inner join date
+on date.id = balance.Balance_Dt_Id 
+where balance.Balance_Dt_Id  = (select max(balance.Balance_Dt_Id)-1 from balance)
+),
+CTE_Daily_Bal_Acct_Type as 
+(
+SELECT client.id as client_id, product.type AS account_type, date.date, date.day, 
+	date.month, date.year, sum(balance.balance) AS balance_acct_type
+ FROM account INNER JOIN product ON account.product_id = product.id 
+ INNER JOIN balance ON account.id = balance.account_id 
+ INNER JOIN date ON balance.balance_dt_id = date.id 
+ INNER JOIN relationship ON account.id = relationship.account_id 
+ INNER JOIN client ON relationship.client_id = client.id  
+WHERE  relationship.relationship_type = 'Primary' 
+GROUP BY client.id, product.type, date.date, date.day, date.month, date.year
+)
+,CTE_MTD_YTD_Avg_Bal as
+(
+SELECT client_id, account_type, date, day, month, year, balance_acct_type
+,avg(balance_acct_type) over (partition by client_id,account_type, year, month order by date) as balance_acct_type_mtd_avg
+,avg(balance_acct_type) over (partition by client_id,account_type, year order by date) as balance_acct_type_ytd_avg
+ FROM CTE_Daily_Bal_Acct_Type
+ order by client_id, account_type, date, day, month, year
+)
+SELECT  date.date, client.id as client_id, product.type AS account_type,  
+ COUNT(CASE WHEN account.status = 'Open' THEN 1 END) AS open_accounts,
+COUNT(CASE WHEN account.status = 'Closed' THEN 1 END) AS closed_accounts, 
+CTE_Daily_Bal_Acct_Type.balance_acct_type AS balance_total_curr
+,CTE_MTD_YTD_Avg_Bal.balance_acct_type_mtd_avg
+ ,CTE_MTD_YTD_Avg_Bal.balance_acct_type_ytd_avg
+ FROM account INNER JOIN product ON account.product_id = product.id 
+ INNER JOIN balance ON account.id = balance.account_id 
+ INNER JOIN date ON balance.balance_dt_id = date.id
+ INNER JOIN relationship ON account.id = relationship.account_id 
+ INNER JOIN client ON relationship.client_id = client.id 
+ inner join CTE_MTD_YTD_Avg_Bal 
+ on 
+ 	CTE_MTD_YTD_Avg_Bal.account_type =  product.type 
+	and CTE_MTD_YTD_Avg_Bal.date = date.date
+	and CTE_MTD_YTD_Avg_Bal.client_id = client.id
+ inner join CTE_Daily_Bal_Acct_Type
+ on 
+ 	CTE_Daily_Bal_Acct_Type.account_type =  product.type 
+	and CTE_Daily_Bal_Acct_Type.date = date.date
+	and CTE_Daily_Bal_Acct_Type.client_id = client.id
+inner JOIN CTE_Latest_Dt
+on CTE_Latest_Dt.date = date.date
+WHERE client.name = 'Robert King'  
+AND relationship.relationship_type = 'Primary'  
+GROUP BY  date.date, client.id, product.type 
+,CTE_Daily_Bal_Acct_Type.balance_acct_type
+,CTE_MTD_YTD_Avg_Bal.balance_acct_type_mtd_avg
+ ,CTE_MTD_YTD_Avg_Bal.balance_acct_type_ytd_avg</t>
+  </si>
+  <si>
+    <t>What is Robert King's current account portfolio?</t>
+  </si>
+  <si>
+    <t>with CTE_Daily_Bal_Acct_Type as 
+(
+SELECT client.id as client_id, product.type AS account_type, date.date, date.day, 
+	date.month, date.year, sum(balance.balance) AS balance_acct_type
+ FROM account INNER JOIN product ON account.product_id = product.id 
+ INNER JOIN balance ON account.id = balance.account_id 
+ INNER JOIN date ON balance.balance_dt_id = date.id 
+ INNER JOIN relationship ON account.id = relationship.account_id 
+ INNER JOIN client ON relationship.client_id = client.id  
+WHERE  relationship.relationship_type = 'Primary' 
+GROUP BY client.id, product.type, date.date, date.day, date.month, date.year
+)
+,CTE_MTD_YTD_Avg_Bal as
+(
+SELECT client_id, account_type, date, day, month, year, balance_acct_type
+,avg(balance_acct_type) over (partition by client_id,account_type, year, month order by date) as balance_acct_type_mtd_avg
+,avg(balance_acct_type) over (partition by client_id,account_type, year order by date) as balance_acct_type_ytd_avg
+ FROM CTE_Daily_Bal_Acct_Type
+ order by client_id, account_type, date, day, month, year
+)
+SELECT  date.date, client.id as client_id, product.type AS account_type,  
+ COUNT(CASE WHEN account.status = 'Open' THEN 1 END) AS open_accounts,
+COUNT(CASE WHEN account.status = 'Closed' THEN 1 END) AS closed_accounts, 
+CTE_Daily_Bal_Acct_Type.balance_acct_type AS balance_total_curr
+,CTE_MTD_YTD_Avg_Bal.balance_acct_type_mtd_avg
+ ,CTE_MTD_YTD_Avg_Bal.balance_acct_type_ytd_avg
+ FROM account INNER JOIN product ON account.product_id = product.id 
+ INNER JOIN balance ON account.id = balance.account_id 
+ INNER JOIN date ON balance.balance_dt_id = date.id
+ INNER JOIN relationship ON account.id = relationship.account_id 
+ INNER JOIN client ON relationship.client_id = client.id 
+ inner join CTE_MTD_YTD_Avg_Bal 
+ on 
+ 	CTE_MTD_YTD_Avg_Bal.account_type =  product.type 
+	and CTE_MTD_YTD_Avg_Bal.date = date.date
+	and CTE_MTD_YTD_Avg_Bal.client_id = client.id
+ inner join CTE_Daily_Bal_Acct_Type
+ on 
+ 	CTE_Daily_Bal_Acct_Type.account_type =  product.type 
+	and CTE_Daily_Bal_Acct_Type.date = date.date
+	and CTE_Daily_Bal_Acct_Type.client_id = client.id
+WHERE client.name = 'Angelica James'  
+AND relationship.relationship_type = 'Primary'  
+and date.date = '2023-08-30'
+GROUP BY  date.date, client.id, product.type 
+,CTE_Daily_Bal_Acct_Type.balance_acct_type
+,CTE_MTD_YTD_Avg_Bal.balance_acct_type_mtd_avg
+ ,CTE_MTD_YTD_Avg_Bal.balance_acct_type_ytd_avg;</t>
+  </si>
+  <si>
+    <t>What is Angelica James account portfolio summary as of 8/30/2023?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +330,12 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -124,10 +374,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -431,13 +685,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D7"/>
+    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="100" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -469,36 +729,116 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
+        <v>34</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="160" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="160" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="176" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="176" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="176" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="208" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="192" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="192" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="208" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>